<commit_message>
fixed score addup rounding
</commit_message>
<xml_diff>
--- a/200530-9-省份平均分统计.xlsx
+++ b/200530-9-省份平均分统计.xlsx
@@ -436,7 +436,7 @@
         <v>267.1</v>
       </c>
       <c r="E2" t="n">
-        <v>511</v>
+        <v>511.2</v>
       </c>
       <c r="G2" t="n">
         <v>9</v>
@@ -448,7 +448,7 @@
         <v>241.7</v>
       </c>
       <c r="J2" t="n">
-        <v>498</v>
+        <v>499.5</v>
       </c>
       <c r="L2" t="n">
         <v>9</v>
@@ -460,7 +460,7 @@
         <v>247.8</v>
       </c>
       <c r="O2" t="n">
-        <v>507</v>
+        <v>507.8</v>
       </c>
     </row>
     <row r="3">
@@ -491,7 +491,7 @@
         <v>267.4</v>
       </c>
       <c r="J3" t="n">
-        <v>497</v>
+        <v>497.4</v>
       </c>
       <c r="L3" t="n">
         <v>21</v>
@@ -503,7 +503,7 @@
         <v>233.6</v>
       </c>
       <c r="O3" t="n">
-        <v>479</v>
+        <v>479.8</v>
       </c>
     </row>
     <row r="4">
@@ -522,7 +522,7 @@
         <v>276.7</v>
       </c>
       <c r="E4" t="n">
-        <v>548</v>
+        <v>549.0999999999999</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>242</v>
       </c>
       <c r="O4" t="n">
-        <v>485</v>
+        <v>485.9</v>
       </c>
     </row>
     <row r="5">
@@ -565,7 +565,7 @@
         <v>214.1</v>
       </c>
       <c r="E5" t="n">
-        <v>457</v>
+        <v>457.2</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -608,7 +608,7 @@
         <v>252.5</v>
       </c>
       <c r="E6" t="n">
-        <v>513</v>
+        <v>514.2</v>
       </c>
       <c r="G6" t="n">
         <v>6</v>
@@ -620,7 +620,7 @@
         <v>259.2</v>
       </c>
       <c r="J6" t="n">
-        <v>521</v>
+        <v>521.7</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -651,7 +651,7 @@
         <v>236.6</v>
       </c>
       <c r="E7" t="n">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>236.4</v>
       </c>
       <c r="O7" t="n">
-        <v>497</v>
+        <v>497.8</v>
       </c>
     </row>
     <row r="8">
@@ -694,7 +694,7 @@
         <v>259.1</v>
       </c>
       <c r="E8" t="n">
-        <v>519</v>
+        <v>519.6</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -718,7 +718,7 @@
         <v>227.4</v>
       </c>
       <c r="O8" t="n">
-        <v>481</v>
+        <v>482.1</v>
       </c>
     </row>
     <row r="9">
@@ -737,7 +737,7 @@
         <v>235.6</v>
       </c>
       <c r="E9" t="n">
-        <v>489</v>
+        <v>489.9</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>205.7</v>
       </c>
       <c r="O9" t="n">
-        <v>469</v>
+        <v>469.8</v>
       </c>
     </row>
     <row r="10">
@@ -780,7 +780,7 @@
         <v>267.3</v>
       </c>
       <c r="E10" t="n">
-        <v>525</v>
+        <v>526.2</v>
       </c>
       <c r="G10" t="n">
         <v>45</v>
@@ -792,7 +792,7 @@
         <v>254.4</v>
       </c>
       <c r="J10" t="n">
-        <v>522</v>
+        <v>522.5</v>
       </c>
       <c r="L10" t="n">
         <v>51</v>
@@ -804,7 +804,7 @@
         <v>252.5</v>
       </c>
       <c r="O10" t="n">
-        <v>495</v>
+        <v>495.9</v>
       </c>
     </row>
     <row r="11">
@@ -823,7 +823,7 @@
         <v>307.4</v>
       </c>
       <c r="E11" t="n">
-        <v>563</v>
+        <v>564.2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>264.4</v>
       </c>
       <c r="J12" t="n">
-        <v>534</v>
+        <v>535.2</v>
       </c>
       <c r="L12" t="n">
         <v>22</v>
@@ -890,7 +890,7 @@
         <v>223.9</v>
       </c>
       <c r="O12" t="n">
-        <v>463</v>
+        <v>464.8</v>
       </c>
     </row>
     <row r="13">
@@ -933,7 +933,7 @@
         <v>235.7</v>
       </c>
       <c r="O13" t="n">
-        <v>472</v>
+        <v>473.1</v>
       </c>
     </row>
     <row r="14">
@@ -952,7 +952,7 @@
         <v>241.3</v>
       </c>
       <c r="E14" t="n">
-        <v>480</v>
+        <v>480.9</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -976,7 +976,7 @@
         <v>254.4</v>
       </c>
       <c r="O14" t="n">
-        <v>510</v>
+        <v>510.8</v>
       </c>
     </row>
     <row r="15">
@@ -995,7 +995,7 @@
         <v>236.5</v>
       </c>
       <c r="E15" t="n">
-        <v>475</v>
+        <v>475.5</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>197.9</v>
       </c>
       <c r="O15" t="n">
-        <v>448</v>
+        <v>449.3</v>
       </c>
     </row>
     <row r="16">
@@ -1038,7 +1038,7 @@
         <v>239.6</v>
       </c>
       <c r="E16" t="n">
-        <v>489</v>
+        <v>489.8</v>
       </c>
       <c r="G16" t="n">
         <v>3</v>
@@ -1050,7 +1050,7 @@
         <v>238.3</v>
       </c>
       <c r="J16" t="n">
-        <v>528</v>
+        <v>528.3</v>
       </c>
       <c r="L16" t="n">
         <v>81</v>
@@ -1062,7 +1062,7 @@
         <v>223.3</v>
       </c>
       <c r="O16" t="n">
-        <v>471</v>
+        <v>471.9</v>
       </c>
     </row>
     <row r="17">
@@ -1093,7 +1093,7 @@
         <v>182.5</v>
       </c>
       <c r="J17" t="n">
-        <v>407</v>
+        <v>407.5</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         <v>216.7</v>
       </c>
       <c r="E18" t="n">
-        <v>453</v>
+        <v>453.7</v>
       </c>
       <c r="G18" t="n">
         <v>187</v>
@@ -1136,7 +1136,7 @@
         <v>243.3</v>
       </c>
       <c r="J18" t="n">
-        <v>492</v>
+        <v>492.3</v>
       </c>
       <c r="L18" t="n">
         <v>62</v>
@@ -1148,7 +1148,7 @@
         <v>245.3</v>
       </c>
       <c r="O18" t="n">
-        <v>493</v>
+        <v>493.9</v>
       </c>
     </row>
     <row r="19">
@@ -1191,7 +1191,7 @@
         <v>260</v>
       </c>
       <c r="O19" t="n">
-        <v>530</v>
+        <v>530.6</v>
       </c>
     </row>
     <row r="20">
@@ -1253,7 +1253,7 @@
         <v>223.2</v>
       </c>
       <c r="E21" t="n">
-        <v>472</v>
+        <v>472.4</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1277,7 +1277,7 @@
         <v>247.5</v>
       </c>
       <c r="O21" t="n">
-        <v>490</v>
+        <v>491.3</v>
       </c>
     </row>
     <row r="22">
@@ -1320,7 +1320,7 @@
         <v>238.2</v>
       </c>
       <c r="O22" t="n">
-        <v>502</v>
+        <v>502.3</v>
       </c>
     </row>
     <row r="23">
@@ -1437,7 +1437,7 @@
         <v>264.3</v>
       </c>
       <c r="J25" t="n">
-        <v>502</v>
+        <v>502.9</v>
       </c>
       <c r="L25" t="n">
         <v>0</v>
@@ -1468,7 +1468,7 @@
         <v>233.8</v>
       </c>
       <c r="E26" t="n">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1523,7 +1523,7 @@
         <v>238.7</v>
       </c>
       <c r="J27" t="n">
-        <v>457</v>
+        <v>458.6</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
@@ -1566,7 +1566,7 @@
         <v>267.5</v>
       </c>
       <c r="J28" t="n">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>242.2</v>
       </c>
       <c r="E29" t="n">
-        <v>473</v>
+        <v>473.9</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1621,7 +1621,7 @@
         <v>213.8</v>
       </c>
       <c r="O29" t="n">
-        <v>451</v>
+        <v>452.1</v>
       </c>
     </row>
     <row r="30">
@@ -1640,7 +1640,7 @@
         <v>248.4</v>
       </c>
       <c r="E30" t="n">
-        <v>507</v>
+        <v>507.5</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1664,7 +1664,7 @@
         <v>244</v>
       </c>
       <c r="O30" t="n">
-        <v>505</v>
+        <v>505.7</v>
       </c>
     </row>
     <row r="31">
@@ -1695,7 +1695,7 @@
         <v>286.8</v>
       </c>
       <c r="J31" t="n">
-        <v>549</v>
+        <v>550.4000000000001</v>
       </c>
       <c r="L31" t="n">
         <v>0</v>
@@ -1738,7 +1738,7 @@
         <v>250.8</v>
       </c>
       <c r="J32" t="n">
-        <v>552</v>
+        <v>553.3</v>
       </c>
       <c r="L32" t="n">
         <v>0</v>
@@ -1793,7 +1793,7 @@
         <v>255.7</v>
       </c>
       <c r="O33" t="n">
-        <v>508</v>
+        <v>508.9</v>
       </c>
     </row>
     <row r="34">

</xml_diff>